<commit_message>
Add average perc errors
</commit_message>
<xml_diff>
--- a/Porovnani_18_04.xlsx
+++ b/Porovnani_18_04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiki\PycharmProjects\Colony_Count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC152000-6AA7-4722-8C0C-F81EFDCC9357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC396826-8A2E-48B3-84C3-F0A27E778628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" activeTab="6" xr2:uid="{48282F01-B452-4B76-B512-DF405AF65261}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="251">
   <si>
     <t>model</t>
   </si>
@@ -741,6 +741,57 @@
   </si>
   <si>
     <t>no FC</t>
+  </si>
+  <si>
+    <t>0,0,1</t>
+  </si>
+  <si>
+    <t>0,1,1</t>
+  </si>
+  <si>
+    <t>1,1,1</t>
+  </si>
+  <si>
+    <t>avg % error</t>
+  </si>
+  <si>
+    <t>90.32184236997774</t>
+  </si>
+  <si>
+    <t>64.13058099218786</t>
+  </si>
+  <si>
+    <t>90.82116015973759</t>
+  </si>
+  <si>
+    <t>62.24938170226276</t>
+  </si>
+  <si>
+    <t>151.46336174798867</t>
+  </si>
+  <si>
+    <t>202.2655959865517</t>
+  </si>
+  <si>
+    <t>194.3026400545786</t>
+  </si>
+  <si>
+    <t>165.82490326348514</t>
+  </si>
+  <si>
+    <t>182.33980927905102</t>
+  </si>
+  <si>
+    <t>112.25514776110376</t>
+  </si>
+  <si>
+    <t>172.90459628290833</t>
+  </si>
+  <si>
+    <t>267.32764299463963</t>
+  </si>
+  <si>
+    <t>68.40943687966862</t>
   </si>
 </sst>
 </file>
@@ -4051,8 +4102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ECBBBA-085B-42F7-910D-6C0032B71C45}">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12410,7 +12461,7 @@
   <dimension ref="A2:N45"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14284,10 +14335,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4847E0A1-974A-4F3D-B06B-051DC59E5772}">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14301,7 +14352,7 @@
     <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14344,8 +14395,11 @@
       <c r="N1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -14388,8 +14442,11 @@
       <c r="N2">
         <v>0.59619</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -14433,7 +14490,7 @@
         <v>0.60183869999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -14477,7 +14534,7 @@
         <v>0.60261564999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -14521,7 +14578,7 @@
         <v>0.60901530000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -14564,8 +14621,11 @@
       <c r="N6">
         <v>0.62757503999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>217</v>
       </c>
@@ -14609,7 +14669,7 @@
         <v>0.62882760000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -14652,8 +14712,11 @@
       <c r="N8">
         <v>0.66936236999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>193</v>
       </c>
@@ -14696,8 +14759,11 @@
       <c r="N9">
         <v>0.76513949999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -14741,7 +14807,7 @@
         <v>0.81664720000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -14785,7 +14851,7 @@
         <v>0.83198340000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -14829,7 +14895,7 @@
         <v>0.86319995000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>195</v>
       </c>
@@ -14872,8 +14938,11 @@
       <c r="N13">
         <v>0.89960669999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -14916,8 +14985,11 @@
       <c r="N14">
         <v>0.93053330000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>189</v>
       </c>
@@ -14960,8 +15032,11 @@
       <c r="N15">
         <v>0.9331545</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -15004,8 +15079,11 @@
       <c r="N16">
         <v>0.95694330000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>186</v>
       </c>
@@ -15048,8 +15126,11 @@
       <c r="N17">
         <v>0.97282769999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>197</v>
       </c>
@@ -15096,7 +15177,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -15139,8 +15220,11 @@
       <c r="N19">
         <v>0.99294954999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>182</v>
       </c>
@@ -15187,7 +15271,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -15230,8 +15314,11 @@
       <c r="N21">
         <v>1.0337512</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -15274,8 +15361,11 @@
       <c r="N22">
         <v>1.0925026</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>208</v>
       </c>
@@ -15318,8 +15408,11 @@
       <c r="N23" s="9">
         <v>1.0948874</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -15362,8 +15455,11 @@
       <c r="N24">
         <v>1.1853804999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>51</v>
       </c>
@@ -15372,7 +15468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>229</v>
       </c>
@@ -15387,7 +15483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28">
         <f>AVERAGE(N2:N9,N19,N23)</f>
         <v>0.718840111</v>
@@ -15397,7 +15493,7 @@
         <v>0.95604821363636361</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -15438,7 +15534,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>945057</v>
       </c>
@@ -15478,8 +15574,15 @@
       <c r="M34">
         <v>0.59619</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P34" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q34">
+        <f>AVERAGE(M35,M37,M38,M43,M44,M45:M47,M49)</f>
+        <v>0.80774828777777774</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>354309</v>
       </c>
@@ -15520,7 +15623,7 @@
         <v>0.60183869999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>77893</v>
       </c>
@@ -15560,8 +15663,15 @@
       <c r="M36">
         <v>0.60261564999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q36">
+        <f>AVERAGE(M34,M36,M39,M41:M42,M48,M51:M52)</f>
+        <v>0.81157713124999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>631621</v>
       </c>
@@ -15602,7 +15712,7 @@
         <v>0.60901530000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>497613</v>
       </c>
@@ -15642,8 +15752,15 @@
       <c r="M38">
         <v>0.62757503999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P38" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q38">
+        <f>AVERAGE(M40,M50,M53:M54)</f>
+        <v>0.98564495499999993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1101</v>
       </c>
@@ -15684,7 +15801,7 @@
         <v>0.62882760000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>651566</v>
       </c>
@@ -15725,7 +15842,7 @@
         <v>0.66936236999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>234858</v>
       </c>
@@ -15766,7 +15883,7 @@
         <v>0.76513949999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>992869</v>
       </c>
@@ -15807,7 +15924,7 @@
         <v>0.81664720000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>200092</v>
       </c>
@@ -15848,7 +15965,7 @@
         <v>0.83198340000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>61565</v>
       </c>
@@ -15889,7 +16006,7 @@
         <v>0.86319995000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>358466</v>
       </c>
@@ -15930,7 +16047,7 @@
         <v>0.89960669999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>593664</v>
       </c>
@@ -15971,7 +16088,7 @@
         <v>0.93053330000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>74054</v>
       </c>
@@ -16012,7 +16129,7 @@
         <v>0.9331545</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>514133</v>
       </c>

</xml_diff>